<commit_message>
Added key values to excel
</commit_message>
<xml_diff>
--- a/key-value.xlsx
+++ b/key-value.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tatiana/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tatiana/Documents/GitHub/glygen-frontend/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98370E78-4C10-684F-B1FA-F0F6174C4A3A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F7B43876-039A-2441-854B-263CDB9E6CF6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="26260" yWindow="460" windowWidth="33920" windowHeight="14180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="27880" yWindow="460" windowWidth="23560" windowHeight="14180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="254">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="256">
   <si>
     <t>Field/Term</t>
   </si>
@@ -476,9 +476,6 @@
     <t>The DNA sequence of human chromosome 7</t>
   </si>
   <si>
-    <t>RefSeq Accession:</t>
-  </si>
-  <si>
     <t>ac</t>
   </si>
   <si>
@@ -677,6 +674,9 @@
     <t>Enter complete or partial GlyTouCan Accession of your glycan (see https://glytoucan.org/)</t>
   </si>
   <si>
+    <t>monoisotopic_mass</t>
+  </si>
+  <si>
     <t>Use the sliders to select a Monoisotopic Mass range for your protein(s)</t>
   </si>
   <si>
@@ -686,10 +686,19 @@
     <t>Use the sliders to select a Number of Sugars range for your protein(s)</t>
   </si>
   <si>
+    <t>glycan_type</t>
+  </si>
+  <si>
     <t>Click to select a Glycan Type</t>
   </si>
   <si>
+    <t>glycan_subtype</t>
+  </si>
+  <si>
     <t>Click to select a Glycan Subtype</t>
+  </si>
+  <si>
+    <t>glycan_motif</t>
   </si>
   <si>
     <t>Enter a Glycan Motif comprising part of your glycan(s)</t>
@@ -817,49 +826,46 @@
     <t>Interacting Glycan</t>
   </si>
   <si>
+    <t>interacting_glycan</t>
+  </si>
+  <si>
     <t>Glycosylated Amino Acid</t>
   </si>
   <si>
-    <t>glycosylated_aa</t>
-  </si>
-  <si>
     <t>Click to highlight multiple selections for Glycosylated Amino Acid</t>
   </si>
   <si>
     <t>Glycosylation Evidences Type</t>
   </si>
   <si>
-    <t>glycosylation_evidence</t>
-  </si>
-  <si>
     <t>Click to select Glycosylation Evidence Type</t>
   </si>
   <si>
-    <t>glycan_id</t>
-  </si>
-  <si>
-    <t>slider sliderbox-slider</t>
-  </si>
-  <si>
-    <t>slider1 sliderbox-slider1</t>
-  </si>
-  <si>
-    <t>protein</t>
-  </si>
-  <si>
-    <t>refseq</t>
-  </si>
-  <si>
-    <t>sequence_type  sequences</t>
-  </si>
-  <si>
-    <t>ddl</t>
-  </si>
-  <si>
-    <t>ddl2</t>
-  </si>
-  <si>
-    <t>motif</t>
+    <t>glycosyl_evidence</t>
+  </si>
+  <si>
+    <t>glycosylated_amino</t>
+  </si>
+  <si>
+    <t>number_sugars</t>
+  </si>
+  <si>
+    <t>uniprot_accession</t>
+  </si>
+  <si>
+    <t>RefSeq Accession</t>
+  </si>
+  <si>
+    <t>refseq_accession</t>
+  </si>
+  <si>
+    <t>protein_sequence</t>
+  </si>
+  <si>
+    <t>glytoucan_accession</t>
+  </si>
+  <si>
+    <t>biosynt_enzyme</t>
   </si>
 </sst>
 </file>
@@ -923,6 +929,12 @@
     </font>
     <font>
       <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -959,16 +971,8 @@
       <family val="2"/>
     </font>
     <font>
-      <b/>
       <sz val="10"/>
-      <color rgb="FFFF0000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color theme="1"/>
+      <color rgb="FF980000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -1011,7 +1015,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -1111,28 +1115,29 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1452,8 +1457,8 @@
   </sheetPr>
   <dimension ref="A1:AD1010"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="149" zoomScaleNormal="179" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="165" zoomScaleNormal="179" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
@@ -1473,16 +1478,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="35" t="s">
-        <v>235</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>213</v>
+        <v>238</v>
+      </c>
+      <c r="C1" s="42" t="s">
+        <v>212</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>2</v>
@@ -1532,14 +1537,14 @@
       <c r="A4" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="43" t="s">
-        <v>13</v>
+      <c r="C4" s="36" t="s">
+        <v>255</v>
       </c>
       <c r="D4" s="13" t="s">
         <v>13</v>
       </c>
       <c r="E4" s="36" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="F4" s="13" t="s">
         <v>14</v>
@@ -1574,14 +1579,14 @@
       <c r="A6" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="42" t="s">
-        <v>246</v>
+      <c r="C6" s="41" t="s">
+        <v>19</v>
       </c>
       <c r="D6" s="14" t="s">
         <v>19</v>
       </c>
       <c r="E6" s="36" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="F6" s="15" t="s">
         <v>20</v>
@@ -1790,14 +1795,14 @@
       <c r="A18" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="C18" s="43" t="s">
-        <v>231</v>
+      <c r="C18" s="36" t="s">
+        <v>234</v>
       </c>
       <c r="D18" s="5" t="s">
         <v>61</v>
       </c>
       <c r="E18" s="36" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="F18" s="5" t="s">
         <v>62</v>
@@ -1830,14 +1835,14 @@
       <c r="A20" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C20" s="43" t="s">
-        <v>253</v>
+      <c r="C20" s="36" t="s">
+        <v>224</v>
       </c>
       <c r="D20" s="14" t="s">
         <v>66</v>
       </c>
       <c r="E20" s="36" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="F20" s="5" t="s">
         <v>67</v>
@@ -1854,14 +1859,14 @@
       <c r="A21" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="C21" s="43" t="s">
-        <v>252</v>
+      <c r="C21" s="36" t="s">
+        <v>222</v>
       </c>
       <c r="D21" s="14" t="s">
         <v>70</v>
       </c>
       <c r="E21" s="36" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="F21" s="5" t="s">
         <v>71</v>
@@ -1878,14 +1883,14 @@
       <c r="A22" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="C22" s="43" t="s">
-        <v>251</v>
+      <c r="C22" s="36" t="s">
+        <v>220</v>
       </c>
       <c r="D22" s="14" t="s">
         <v>74</v>
       </c>
       <c r="E22" s="36" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="F22" s="5" t="s">
         <v>75</v>
@@ -1973,16 +1978,16 @@
         <v>88</v>
       </c>
       <c r="B27" s="36" t="s">
-        <v>215</v>
-      </c>
-      <c r="C27" s="43" t="s">
-        <v>245</v>
+        <v>214</v>
+      </c>
+      <c r="C27" s="36" t="s">
+        <v>254</v>
       </c>
       <c r="D27" s="14" t="s">
         <v>89</v>
       </c>
       <c r="E27" s="36" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F27" s="5" t="s">
         <v>90</v>
@@ -2069,8 +2074,8 @@
       <c r="A32" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="C32" s="42" t="s">
-        <v>246</v>
+      <c r="C32" s="41" t="s">
+        <v>216</v>
       </c>
       <c r="D32" s="14" t="s">
         <v>109</v>
@@ -2142,14 +2147,14 @@
       <c r="A36" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="C36" s="43" t="s">
+      <c r="C36" s="36" t="s">
         <v>119</v>
       </c>
       <c r="D36" s="14" t="s">
         <v>119</v>
       </c>
       <c r="E36" s="36" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="F36" s="5" t="s">
         <v>120</v>
@@ -2184,14 +2189,14 @@
       <c r="A38" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="C38" s="43" t="s">
+      <c r="C38" s="36" t="s">
         <v>125</v>
       </c>
       <c r="D38" s="5" t="s">
         <v>125</v>
       </c>
       <c r="E38" s="36" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="F38" s="5" t="s">
         <v>126</v>
@@ -2277,14 +2282,14 @@
       <c r="A43" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="C43" s="43" t="s">
-        <v>229</v>
+      <c r="C43" s="36" t="s">
+        <v>232</v>
       </c>
       <c r="D43" s="14" t="s">
         <v>139</v>
       </c>
       <c r="E43" s="36" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="F43" s="5" t="s">
         <v>140</v>
@@ -2302,16 +2307,16 @@
         <v>142</v>
       </c>
       <c r="B44" s="36" t="s">
-        <v>234</v>
-      </c>
-      <c r="C44" s="42" t="s">
-        <v>250</v>
+        <v>237</v>
+      </c>
+      <c r="C44" s="43" t="s">
+        <v>253</v>
       </c>
       <c r="D44" s="5" t="s">
         <v>143</v>
       </c>
       <c r="E44" s="36" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="F44" s="5" t="s">
         <v>144</v>
@@ -2343,26 +2348,26 @@
       <c r="I45" s="8"/>
     </row>
     <row r="46" spans="1:9" ht="28">
-      <c r="A46" s="4" t="s">
+      <c r="A46" s="39" t="s">
+        <v>251</v>
+      </c>
+      <c r="B46" s="36" t="s">
+        <v>228</v>
+      </c>
+      <c r="C46" s="36" t="s">
+        <v>252</v>
+      </c>
+      <c r="D46" s="14" t="s">
         <v>150</v>
       </c>
-      <c r="B46" s="36" t="s">
-        <v>225</v>
-      </c>
-      <c r="C46" s="43" t="s">
-        <v>249</v>
-      </c>
-      <c r="D46" s="14" t="s">
+      <c r="E46" s="36" t="s">
+        <v>229</v>
+      </c>
+      <c r="F46" s="5" t="s">
         <v>151</v>
       </c>
-      <c r="E46" s="36" t="s">
-        <v>226</v>
-      </c>
-      <c r="F46" s="5" t="s">
+      <c r="G46" s="6" t="s">
         <v>152</v>
-      </c>
-      <c r="G46" s="6" t="s">
-        <v>153</v>
       </c>
       <c r="H46" s="7" t="s">
         <v>9</v>
@@ -2371,16 +2376,16 @@
     </row>
     <row r="47" spans="1:9" ht="28">
       <c r="A47" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="D47" s="14" t="s">
         <v>154</v>
       </c>
-      <c r="D47" s="14" t="s">
+      <c r="F47" s="5" t="s">
         <v>155</v>
       </c>
-      <c r="F47" s="5" t="s">
+      <c r="G47" s="6" t="s">
         <v>156</v>
-      </c>
-      <c r="G47" s="6" t="s">
-        <v>157</v>
       </c>
       <c r="H47" s="7" t="s">
         <v>9</v>
@@ -2389,13 +2394,13 @@
     </row>
     <row r="48" spans="1:9" ht="14">
       <c r="A48" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D48" s="5" t="s">
         <v>6</v>
       </c>
       <c r="F48" s="5" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="G48" s="20"/>
       <c r="H48" s="7" t="s">
@@ -2405,16 +2410,16 @@
     </row>
     <row r="49" spans="1:30" ht="14">
       <c r="A49" s="17" t="s">
+        <v>159</v>
+      </c>
+      <c r="D49" s="14" t="s">
         <v>160</v>
       </c>
-      <c r="D49" s="14" t="s">
+      <c r="F49" s="18" t="s">
         <v>161</v>
       </c>
-      <c r="F49" s="18" t="s">
+      <c r="G49" s="14" t="s">
         <v>162</v>
-      </c>
-      <c r="G49" s="14" t="s">
-        <v>163</v>
       </c>
       <c r="H49" s="7" t="s">
         <v>9</v>
@@ -2422,16 +2427,16 @@
     </row>
     <row r="50" spans="1:30" ht="28">
       <c r="A50" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="D50" s="5" t="s">
         <v>164</v>
       </c>
-      <c r="D50" s="5" t="s">
+      <c r="F50" s="5" t="s">
         <v>165</v>
       </c>
-      <c r="F50" s="5" t="s">
+      <c r="G50" s="6" t="s">
         <v>166</v>
-      </c>
-      <c r="G50" s="6" t="s">
-        <v>167</v>
       </c>
       <c r="H50" s="7" t="s">
         <v>9</v>
@@ -2440,16 +2445,16 @@
     </row>
     <row r="51" spans="1:30" ht="14">
       <c r="A51" s="4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D51" s="14" t="s">
         <v>61</v>
       </c>
       <c r="F51" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="G51" s="6" t="s">
         <v>169</v>
-      </c>
-      <c r="G51" s="6" t="s">
-        <v>170</v>
       </c>
       <c r="H51" s="7" t="s">
         <v>9</v>
@@ -2458,13 +2463,13 @@
     </row>
     <row r="52" spans="1:30" ht="14">
       <c r="A52" s="17" t="s">
+        <v>170</v>
+      </c>
+      <c r="D52" s="14" t="s">
         <v>171</v>
       </c>
-      <c r="D52" s="14" t="s">
+      <c r="F52" s="18" t="s">
         <v>172</v>
-      </c>
-      <c r="F52" s="18" t="s">
-        <v>173</v>
       </c>
       <c r="G52" s="14">
         <v>700</v>
@@ -2475,13 +2480,13 @@
     </row>
     <row r="53" spans="1:30" ht="14">
       <c r="A53" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="D53" s="14" t="s">
         <v>174</v>
       </c>
-      <c r="D53" s="14" t="s">
+      <c r="F53" s="5" t="s">
         <v>175</v>
-      </c>
-      <c r="F53" s="5" t="s">
-        <v>176</v>
       </c>
       <c r="G53" s="6">
         <v>9606</v>
@@ -2493,16 +2498,16 @@
     </row>
     <row r="54" spans="1:30" ht="13">
       <c r="A54" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D54" s="14" t="s">
         <v>6</v>
       </c>
       <c r="F54" s="14" t="s">
+        <v>177</v>
+      </c>
+      <c r="G54" s="6" t="s">
         <v>178</v>
-      </c>
-      <c r="G54" s="6" t="s">
-        <v>179</v>
       </c>
       <c r="H54" s="7" t="s">
         <v>9</v>
@@ -2511,16 +2516,16 @@
     </row>
     <row r="55" spans="1:30" ht="14">
       <c r="A55" s="17" t="s">
+        <v>179</v>
+      </c>
+      <c r="D55" s="18" t="s">
         <v>180</v>
       </c>
-      <c r="D55" s="18" t="s">
+      <c r="F55" s="18" t="s">
         <v>181</v>
       </c>
-      <c r="F55" s="18" t="s">
+      <c r="G55" s="14" t="s">
         <v>182</v>
-      </c>
-      <c r="G55" s="14" t="s">
-        <v>183</v>
       </c>
       <c r="H55" s="7" t="s">
         <v>9</v>
@@ -2528,16 +2533,16 @@
     </row>
     <row r="56" spans="1:30" ht="14">
       <c r="A56" s="17" t="s">
+        <v>183</v>
+      </c>
+      <c r="D56" s="14" t="s">
         <v>184</v>
       </c>
-      <c r="D56" s="14" t="s">
+      <c r="F56" s="18" t="s">
         <v>185</v>
       </c>
-      <c r="F56" s="18" t="s">
+      <c r="G56" s="14" t="s">
         <v>186</v>
-      </c>
-      <c r="G56" s="14" t="s">
-        <v>187</v>
       </c>
       <c r="H56" s="7" t="s">
         <v>9</v>
@@ -2545,16 +2550,16 @@
     </row>
     <row r="57" spans="1:30" ht="14">
       <c r="A57" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="D57" s="5" t="s">
         <v>188</v>
       </c>
-      <c r="D57" s="5" t="s">
+      <c r="F57" s="5" t="s">
         <v>189</v>
       </c>
-      <c r="F57" s="5" t="s">
+      <c r="G57" s="6" t="s">
         <v>190</v>
-      </c>
-      <c r="G57" s="6" t="s">
-        <v>191</v>
       </c>
       <c r="H57" s="7" t="s">
         <v>9</v>
@@ -2563,25 +2568,25 @@
     </row>
     <row r="58" spans="1:30" ht="32">
       <c r="A58" s="39" t="s">
+        <v>191</v>
+      </c>
+      <c r="B58" s="36" t="s">
+        <v>213</v>
+      </c>
+      <c r="C58" s="43" t="s">
+        <v>250</v>
+      </c>
+      <c r="D58" s="14" t="s">
         <v>192</v>
       </c>
-      <c r="B58" s="36" t="s">
-        <v>214</v>
-      </c>
-      <c r="C58" s="44" t="s">
-        <v>248</v>
-      </c>
-      <c r="D58" s="14" t="s">
+      <c r="E58" s="36" t="s">
+        <v>227</v>
+      </c>
+      <c r="F58" s="40" t="s">
         <v>193</v>
       </c>
-      <c r="E58" s="36" t="s">
-        <v>224</v>
-      </c>
-      <c r="F58" s="40" t="s">
+      <c r="G58" s="16" t="s">
         <v>194</v>
-      </c>
-      <c r="G58" s="16" t="s">
-        <v>195</v>
       </c>
       <c r="H58" s="22" t="s">
         <v>9</v>
@@ -2590,16 +2595,16 @@
     </row>
     <row r="59" spans="1:30" ht="28">
       <c r="A59" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="D59" s="5" t="s">
         <v>196</v>
       </c>
-      <c r="D59" s="5" t="s">
+      <c r="F59" s="5" t="s">
         <v>197</v>
       </c>
-      <c r="F59" s="5" t="s">
+      <c r="G59" s="41" t="s">
         <v>198</v>
-      </c>
-      <c r="G59" s="41" t="s">
-        <v>199</v>
       </c>
       <c r="H59" s="7" t="s">
         <v>9</v>
@@ -2608,16 +2613,16 @@
     </row>
     <row r="60" spans="1:30" ht="14">
       <c r="A60" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="D60" s="14" t="s">
         <v>200</v>
       </c>
-      <c r="D60" s="14" t="s">
+      <c r="F60" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="F60" s="5" t="s">
+      <c r="G60" s="6" t="s">
         <v>202</v>
-      </c>
-      <c r="G60" s="6" t="s">
-        <v>203</v>
       </c>
       <c r="H60" s="7" t="s">
         <v>9</v>
@@ -2630,10 +2635,10 @@
       </c>
       <c r="B61" s="28"/>
       <c r="D61" s="25" t="s">
+        <v>203</v>
+      </c>
+      <c r="F61" s="26" t="s">
         <v>204</v>
-      </c>
-      <c r="F61" s="26" t="s">
-        <v>205</v>
       </c>
       <c r="G61" s="27" t="s">
         <v>6</v>
@@ -2670,10 +2675,10 @@
       </c>
       <c r="B62" s="28"/>
       <c r="D62" s="25" t="s">
+        <v>205</v>
+      </c>
+      <c r="F62" s="26" t="s">
         <v>206</v>
-      </c>
-      <c r="F62" s="26" t="s">
-        <v>207</v>
       </c>
       <c r="G62" s="27" t="s">
         <v>6</v>
@@ -2710,10 +2715,10 @@
       </c>
       <c r="B63" s="28"/>
       <c r="D63" s="29" t="s">
+        <v>207</v>
+      </c>
+      <c r="F63" s="26" t="s">
         <v>208</v>
-      </c>
-      <c r="F63" s="26" t="s">
-        <v>209</v>
       </c>
       <c r="G63" s="27">
         <v>1125</v>
@@ -2750,10 +2755,10 @@
       </c>
       <c r="B64" s="28"/>
       <c r="D64" s="29" t="s">
+        <v>209</v>
+      </c>
+      <c r="F64" s="26" t="s">
         <v>210</v>
-      </c>
-      <c r="F64" s="26" t="s">
-        <v>211</v>
       </c>
       <c r="G64" s="27" t="s">
         <v>6</v>
@@ -2802,8 +2807,8 @@
       <c r="A67" s="39" t="s">
         <v>218</v>
       </c>
-      <c r="C67" s="42" t="s">
-        <v>247</v>
+      <c r="C67" s="41" t="s">
+        <v>249</v>
       </c>
       <c r="D67" s="32"/>
       <c r="E67" s="36" t="s">
@@ -2815,14 +2820,14 @@
     </row>
     <row r="68" spans="1:8" ht="13">
       <c r="A68" s="39" t="s">
-        <v>238</v>
-      </c>
-      <c r="C68" s="42" t="s">
-        <v>245</v>
+        <v>241</v>
+      </c>
+      <c r="C68" s="43" t="s">
+        <v>242</v>
       </c>
       <c r="D68" s="32"/>
       <c r="E68" s="36" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="F68" s="32"/>
       <c r="G68" s="33"/>
@@ -2830,14 +2835,14 @@
     </row>
     <row r="69" spans="1:8" ht="13">
       <c r="A69" s="39" t="s">
-        <v>239</v>
-      </c>
-      <c r="C69" s="43" t="s">
-        <v>240</v>
+        <v>243</v>
+      </c>
+      <c r="C69" s="36" t="s">
+        <v>248</v>
       </c>
       <c r="D69" s="32"/>
       <c r="E69" s="36" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="F69" s="32"/>
       <c r="G69" s="33"/>
@@ -2845,14 +2850,14 @@
     </row>
     <row r="70" spans="1:8" ht="13">
       <c r="A70" s="39" t="s">
-        <v>242</v>
-      </c>
-      <c r="C70" s="43" t="s">
-        <v>243</v>
+        <v>245</v>
+      </c>
+      <c r="C70" s="36" t="s">
+        <v>247</v>
       </c>
       <c r="D70" s="32"/>
       <c r="E70" s="36" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="F70" s="32"/>
       <c r="G70" s="33"/>

</xml_diff>

<commit_message>
Js doc for documentation
</commit_message>
<xml_diff>
--- a/key-value.xlsx
+++ b/key-value.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000"/>
+    <workbookView xWindow="1280" yWindow="780" windowWidth="28800" windowHeight="16580"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1565,7 +1565,7 @@
   </sheetPr>
   <dimension ref="A1:AD1008"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A54" zoomScale="165" zoomScaleNormal="179" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="165" zoomScaleNormal="179" workbookViewId="0">
       <selection activeCell="F57" sqref="F57:H57"/>
     </sheetView>
   </sheetViews>

</xml_diff>